<commit_message>
add technical well statuses
</commit_message>
<xml_diff>
--- a/public/technical_well_forecast.xlsx
+++ b/public/technical_well_forecast.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Дата</t>
   </si>
@@ -32,37 +32,43 @@
     <t>Скважина</t>
   </si>
   <si>
-    <t>нефть факт</t>
-  </si>
-  <si>
     <t>Жидкость факт</t>
   </si>
   <si>
-    <t>отр время</t>
-  </si>
-  <si>
-    <t>Время простоя</t>
-  </si>
-  <si>
     <t>Доли ПРС</t>
   </si>
   <si>
-    <t>нефть прогноз</t>
-  </si>
-  <si>
     <t>Потери нефти</t>
   </si>
   <si>
-    <t>жидкость прогноз</t>
-  </si>
-  <si>
     <t>Потери жидкости</t>
   </si>
   <si>
-    <t>Тех потери нефть</t>
-  </si>
-  <si>
-    <t>Тех потери Жидкость</t>
+    <t>Состояние</t>
+  </si>
+  <si>
+    <t>Причина потерь</t>
+  </si>
+  <si>
+    <t>Нефть факт</t>
+  </si>
+  <si>
+    <t>Нефть прогноз</t>
+  </si>
+  <si>
+    <t>Жидкость прогноз</t>
+  </si>
+  <si>
+    <t>Тех потери нефти</t>
+  </si>
+  <si>
+    <t>Тех потери жидкости</t>
+  </si>
+  <si>
+    <t>Отработанные часы</t>
+  </si>
+  <si>
+    <t>Часы в простое</t>
   </si>
 </sst>
 </file>
@@ -422,20 +428,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N1"/>
+  <dimension ref="A1:P1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="14" width="11.140625" style="2" customWidth="1"/>
+    <col min="1" max="4" width="11.140625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="21.5703125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" style="2" customWidth="1"/>
+    <col min="7" max="8" width="11.140625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="16.28515625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="11.140625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="12.28515625" style="2" customWidth="1"/>
+    <col min="12" max="12" width="19" style="2" customWidth="1"/>
+    <col min="13" max="13" width="16.5703125" style="2" customWidth="1"/>
+    <col min="14" max="14" width="15.85546875" style="2" customWidth="1"/>
     <col min="15" max="15" width="19.140625" style="2" customWidth="1"/>
     <col min="16" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
@@ -443,39 +458,45 @@
         <v>0</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>3</v>
-      </c>
       <c r="E1" s="4" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="4" t="s">
         <v>7</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>8</v>
       </c>
       <c r="J1" s="4" t="s">
         <v>9</v>
       </c>
       <c r="K1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="L1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="M1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="N1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="3"/>
+      <c r="P1" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>